<commit_message>
done 1a using selenide, with parallel execution
</commit_message>
<xml_diff>
--- a/src/test/resource/assignment_test.xlsx
+++ b/src/test/resource/assignment_test.xlsx
@@ -16,7 +16,7 @@
     <t>shoes</t>
   </si>
   <si>
-    <t>Price -- Low to High</t>
+    <t>Low to High</t>
   </si>
 </sst>
 </file>
@@ -282,7 +282,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="14.43"/>
+    <col customWidth="1" min="1" max="1" width="14.43"/>
+    <col customWidth="1" min="2" max="2" width="19.0"/>
+    <col customWidth="1" min="3" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">

</xml_diff>